<commit_message>
metrics start & Hauteur rework commit 24/03/25
</commit_message>
<xml_diff>
--- a/Data/Data placettes/DATA_placette_CANOPIX/Hauteurs_arbres_pieges_2024.xlsx
+++ b/Data/Data placettes/DATA_placette_CANOPIX/Hauteurs_arbres_pieges_2024.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\NO-DATAFILE\Biodiversite\projets\Bois_mort\Canopee\These_Balvay\Data\Campagne 2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adebout\Desktop\Adrien Debout Stage\STATS\Stats_coleo_AD\Data\Data placettes\DATA_placette_CANOPIX\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7380" windowHeight="550"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7380" windowHeight="552"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -505,20 +505,20 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.81640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1796875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="9.6328125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="14.08984375" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.08984375" style="7" customWidth="1"/>
-    <col min="6" max="9" width="14.08984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" style="7" customWidth="1"/>
+    <col min="6" max="9" width="14.109375" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -547,7 +547,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -576,7 +576,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -605,7 +605,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -634,7 +634,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -663,7 +663,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -692,7 +692,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -721,7 +721,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -750,7 +750,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -779,7 +779,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -808,7 +808,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -825,7 +825,7 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
@@ -854,7 +854,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
@@ -883,7 +883,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>21</v>
       </c>
@@ -912,7 +912,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>21</v>
       </c>
@@ -941,7 +941,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>21</v>
       </c>
@@ -970,7 +970,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>21</v>
       </c>
@@ -999,7 +999,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>12.6</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
calculs metriques seuils et début BMP 25/03/25
</commit_message>
<xml_diff>
--- a/Data/Data placettes/DATA_placette_CANOPIX/Hauteurs_arbres_pieges_2024.xlsx
+++ b/Data/Data placettes/DATA_placette_CANOPIX/Hauteurs_arbres_pieges_2024.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adebout\Desktop\Adrien Debout Stage\STATS\Stats_coleo_AD\Data\Data placettes\DATA_placette_CANOPIX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\NO-DATAFILE\Biodiversite\projets\Bois_mort\Canopee\These_Balvay\Data\Campagne 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7380" windowHeight="552"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7380" windowHeight="550"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -505,20 +505,20 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.77734375" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" style="7" customWidth="1"/>
-    <col min="6" max="9" width="14.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.81640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1796875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="9.6328125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="14.08984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.08984375" style="7" customWidth="1"/>
+    <col min="6" max="9" width="14.08984375" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -547,7 +547,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -576,7 +576,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -605,7 +605,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -634,7 +634,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -663,7 +663,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -692,7 +692,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -721,7 +721,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -750,7 +750,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -779,7 +779,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -808,7 +808,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -818,14 +818,20 @@
       <c r="C11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="D11" s="5">
+        <v>38</v>
+      </c>
+      <c r="E11" s="5">
+        <v>36</v>
+      </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
+      <c r="H11" s="5">
+        <v>15.1</v>
+      </c>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
@@ -854,7 +860,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
@@ -883,7 +889,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>21</v>
       </c>
@@ -912,7 +918,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>21</v>
       </c>
@@ -941,7 +947,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>21</v>
       </c>
@@ -970,7 +976,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>21</v>
       </c>
@@ -999,7 +1005,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -1028,7 +1034,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
@@ -1057,7 +1063,7 @@
         <v>12.6</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
@@ -1086,7 +1092,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>

</xml_diff>